<commit_message>
img files are now located in the images file
</commit_message>
<xml_diff>
--- a/cinefilia.xlsx
+++ b/cinefilia.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\git\sites\filmes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\git\filmeTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26278120-0314-4D14-8D84-7E59D7EED17E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A745C32B-5E35-4E42-934D-42A18D92817B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9420" xr2:uid="{946EF7EE-034E-4F7F-BB1F-D7E396B82FD7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{946EF7EE-034E-4F7F-BB1F-D7E396B82FD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -464,7 +464,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
now the rating is out of 5, with classifition in division, with .5
</commit_message>
<xml_diff>
--- a/cinefilia.xlsx
+++ b/cinefilia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\git\filmeTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8749E5-28DC-4F21-859C-3A07E31C7FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A686BC8A-F385-4A40-92DF-8B6AC5914B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{946EF7EE-034E-4F7F-BB1F-D7E396B82FD7}"/>
   </bookViews>
@@ -476,7 +476,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -509,7 +509,7 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>3.5</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -529,7 +529,7 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -549,7 +549,7 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>9</v>
+        <v>4.5</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -569,7 +569,7 @@
         <v>16</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -589,7 +589,7 @@
         <v>19</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
more movies with covers
</commit_message>
<xml_diff>
--- a/cinefilia.xlsx
+++ b/cinefilia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\git\filmeTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7FBC45-F052-441C-84DA-8F015D71E4C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7E2F7B-4E7D-445A-A4DF-4C0F6F4F5111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{946EF7EE-034E-4F7F-BB1F-D7E396B82FD7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{946EF7EE-034E-4F7F-BB1F-D7E396B82FD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="275">
   <si>
     <t>nome</t>
   </si>
@@ -110,21 +110,12 @@
     <t>curta</t>
   </si>
   <si>
-    <t>hideous</t>
-  </si>
-  <si>
     <t>This was probably my favorite thing i watched on Motel X, it was really funny and disturbing, loved it. WHEN HE STARTED SUCKING, OMG, COULDN'T STOP LAUGHING.</t>
   </si>
   <si>
-    <t>blood_dinossaurs</t>
-  </si>
-  <si>
     <t>curtas</t>
   </si>
   <si>
-    <t>heathers</t>
-  </si>
-  <si>
     <t>DARLING in the FRANXX</t>
   </si>
   <si>
@@ -819,13 +810,64 @@
   </si>
   <si>
     <t>1.5</t>
+  </si>
+  <si>
+    <t>guardioes_galaxia</t>
+  </si>
+  <si>
+    <t>interstellar</t>
+  </si>
+  <si>
+    <t>soul_historia</t>
+  </si>
+  <si>
+    <t>alice_pais_maravilhas</t>
+  </si>
+  <si>
+    <t>charlie_chocolate</t>
+  </si>
+  <si>
+    <t>wonka</t>
+  </si>
+  <si>
+    <t>barbie_real</t>
+  </si>
+  <si>
+    <t>variacoes</t>
+  </si>
+  <si>
+    <t>dragao_desejo</t>
+  </si>
+  <si>
+    <t>witcher_night</t>
+  </si>
+  <si>
+    <t>brave_indomavel</t>
+  </si>
+  <si>
+    <t>monstros_uni</t>
+  </si>
+  <si>
+    <t>procura_dori</t>
+  </si>
+  <si>
+    <t>incredibles_2</t>
+  </si>
+  <si>
+    <t>forca_ralph</t>
+  </si>
+  <si>
+    <t>baymax</t>
+  </si>
+  <si>
+    <t>ralph_vs_internet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1192,13 +1234,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EEC174D-8F53-4220-8FB7-8A386CA83EB4}">
   <dimension ref="A1:H120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="D113" sqref="D113"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1221,10 +1263,10 @@
         <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1232,13 +1274,13 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
@@ -1247,12 +1289,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1261,7 +1303,7 @@
         <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
@@ -1270,7 +1312,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1278,7 +1320,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -1293,7 +1335,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1307,7 +1349,7 @@
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -1316,7 +1358,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1330,7 +1372,7 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F6" t="s">
         <v>15</v>
@@ -1339,12 +1381,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -1353,44 +1395,44 @@
         <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>258</v>
       </c>
       <c r="G7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C8">
         <v>5</v>
       </c>
       <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>145</v>
+      </c>
+      <c r="F8" t="s">
+        <v>259</v>
+      </c>
+      <c r="G8" t="s">
         <v>25</v>
       </c>
-      <c r="E8" t="s">
-        <v>148</v>
-      </c>
-      <c r="F8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C9">
         <v>4</v>
@@ -1399,22 +1441,22 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>260</v>
       </c>
       <c r="G9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>A9 + 1</f>
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C10">
         <v>4</v>
@@ -1423,46 +1465,46 @@
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F10" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="G10" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ref="A11:A74" si="0">A10 + 1</f>
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F11" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
       <c r="G11" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C12">
         <v>4</v>
@@ -1471,94 +1513,94 @@
         <v>7</v>
       </c>
       <c r="E12" t="s">
+        <v>149</v>
+      </c>
+      <c r="F12" t="s">
+        <v>263</v>
+      </c>
+      <c r="G12" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>253</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>150</v>
+      </c>
+      <c r="F13" t="s">
+        <v>264</v>
+      </c>
+      <c r="G13" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>255</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>151</v>
+      </c>
+      <c r="F14" t="s">
+        <v>265</v>
+      </c>
+      <c r="G14" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
+        <v>253</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
         <v>152</v>
       </c>
-      <c r="F12" t="s">
-        <v>253</v>
-      </c>
-      <c r="G12" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="F15" t="s">
+        <v>266</v>
+      </c>
+      <c r="G15" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>36</v>
-      </c>
-      <c r="C13" t="s">
-        <v>256</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" t="s">
-        <v>153</v>
-      </c>
-      <c r="F13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G13" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" t="s">
-        <v>258</v>
-      </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" t="s">
-        <v>154</v>
-      </c>
-      <c r="F14" t="s">
-        <v>253</v>
-      </c>
-      <c r="G14" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" t="s">
-        <v>256</v>
-      </c>
-      <c r="D15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" t="s">
-        <v>155</v>
-      </c>
-      <c r="F15" t="s">
-        <v>253</v>
-      </c>
-      <c r="G15" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>39</v>
       </c>
       <c r="C16">
         <v>4</v>
@@ -1567,22 +1609,22 @@
         <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F16" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
       <c r="G16" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C17">
         <v>4</v>
@@ -1591,70 +1633,70 @@
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F17" t="s">
+        <v>268</v>
+      </c>
+      <c r="G17" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
         <v>253</v>
       </c>
-      <c r="G17" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" t="s">
-        <v>256</v>
-      </c>
       <c r="D18" t="s">
         <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F18" t="s">
+        <v>269</v>
+      </c>
+      <c r="G18" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
         <v>253</v>
       </c>
-      <c r="G18" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" t="s">
-        <v>256</v>
-      </c>
       <c r="D19" t="s">
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F19" t="s">
-        <v>253</v>
+        <v>270</v>
       </c>
       <c r="G19" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C20">
         <v>4</v>
@@ -1663,22 +1705,22 @@
         <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F20" t="s">
-        <v>253</v>
+        <v>271</v>
       </c>
       <c r="G20" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C21">
         <v>4</v>
@@ -1687,22 +1729,22 @@
         <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F21" t="s">
-        <v>253</v>
+        <v>272</v>
       </c>
       <c r="G21" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C22">
         <v>5</v>
@@ -1711,46 +1753,46 @@
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F22" t="s">
+        <v>273</v>
+      </c>
+      <c r="G22" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" t="s">
         <v>253</v>
       </c>
-      <c r="G22" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" t="s">
-        <v>256</v>
-      </c>
       <c r="D23" t="s">
         <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F23" t="s">
-        <v>253</v>
+        <v>274</v>
       </c>
       <c r="G23" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C24">
         <v>4</v>
@@ -1759,46 +1801,46 @@
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F24" t="s">
+        <v>250</v>
+      </c>
+      <c r="G24" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" t="s">
         <v>253</v>
       </c>
-      <c r="G24" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" t="s">
-        <v>256</v>
-      </c>
       <c r="D25" t="s">
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F25" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G25" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C26">
         <v>4</v>
@@ -1807,22 +1849,22 @@
         <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F26" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G26" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C27">
         <v>4</v>
@@ -1831,22 +1873,22 @@
         <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F27" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G27" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C28">
         <v>3</v>
@@ -1855,22 +1897,22 @@
         <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F28" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G28" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C29">
         <v>3</v>
@@ -1879,46 +1921,46 @@
         <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F29" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G29" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D30" t="s">
         <v>7</v>
       </c>
       <c r="E30" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F30" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G30" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C31">
         <v>3</v>
@@ -1927,46 +1969,46 @@
         <v>7</v>
       </c>
       <c r="E31" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F31" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G31" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D32" t="s">
         <v>7</v>
       </c>
       <c r="E32" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F32" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G32" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C33">
         <v>3</v>
@@ -1975,46 +2017,46 @@
         <v>7</v>
       </c>
       <c r="E33" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F33" t="s">
+        <v>250</v>
+      </c>
+      <c r="G33" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" t="s">
         <v>253</v>
       </c>
-      <c r="G33" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" t="s">
-        <v>256</v>
-      </c>
       <c r="D34" t="s">
         <v>7</v>
       </c>
       <c r="E34" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F34" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G34" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C35">
         <v>4</v>
@@ -2023,22 +2065,22 @@
         <v>7</v>
       </c>
       <c r="E35" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F35" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G35" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -2047,22 +2089,22 @@
         <v>7</v>
       </c>
       <c r="E36" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F36" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G36" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C37">
         <v>4</v>
@@ -2071,22 +2113,22 @@
         <v>7</v>
       </c>
       <c r="E37" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F37" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G37" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C38">
         <v>4</v>
@@ -2095,22 +2137,22 @@
         <v>7</v>
       </c>
       <c r="E38" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F38" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G38" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C39">
         <v>3</v>
@@ -2119,46 +2161,46 @@
         <v>7</v>
       </c>
       <c r="E39" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F39" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G39" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="B40" t="s">
-        <v>63</v>
-      </c>
-      <c r="C40" t="s">
-        <v>257</v>
-      </c>
       <c r="D40" t="s">
         <v>7</v>
       </c>
       <c r="E40" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F40" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G40" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C41">
         <v>3</v>
@@ -2167,166 +2209,166 @@
         <v>7</v>
       </c>
       <c r="E41" t="s">
+        <v>177</v>
+      </c>
+      <c r="F41" t="s">
+        <v>250</v>
+      </c>
+      <c r="G41" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" t="s">
+        <v>253</v>
+      </c>
+      <c r="D42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" t="s">
+        <v>178</v>
+      </c>
+      <c r="F42" t="s">
+        <v>250</v>
+      </c>
+      <c r="G42" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43" t="s">
+        <v>253</v>
+      </c>
+      <c r="D43" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" t="s">
+        <v>179</v>
+      </c>
+      <c r="F43" t="s">
+        <v>250</v>
+      </c>
+      <c r="G43" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" t="s">
+        <v>253</v>
+      </c>
+      <c r="D44" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" t="s">
         <v>180</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F44" t="s">
+        <v>250</v>
+      </c>
+      <c r="G44" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>65</v>
+      </c>
+      <c r="C45" t="s">
         <v>253</v>
       </c>
-      <c r="G41" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="B42" t="s">
-        <v>65</v>
-      </c>
-      <c r="C42" t="s">
-        <v>256</v>
-      </c>
-      <c r="D42" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="D45" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" t="s">
         <v>181</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F45" t="s">
+        <v>250</v>
+      </c>
+      <c r="G45" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>66</v>
+      </c>
+      <c r="C46" t="s">
         <v>253</v>
       </c>
-      <c r="G42" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="B43" t="s">
-        <v>66</v>
-      </c>
-      <c r="C43" t="s">
-        <v>256</v>
-      </c>
-      <c r="D43" t="s">
-        <v>7</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="D46" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" t="s">
         <v>182</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F46" t="s">
+        <v>250</v>
+      </c>
+      <c r="G46" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>67</v>
+      </c>
+      <c r="C47" t="s">
         <v>253</v>
       </c>
-      <c r="G43" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="B44" t="s">
-        <v>67</v>
-      </c>
-      <c r="C44" t="s">
-        <v>256</v>
-      </c>
-      <c r="D44" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" t="s">
+      <c r="D47" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" t="s">
         <v>183</v>
       </c>
-      <c r="F44" t="s">
-        <v>253</v>
-      </c>
-      <c r="G44" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="B45" t="s">
+      <c r="F47" t="s">
+        <v>250</v>
+      </c>
+      <c r="G47" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
         <v>68</v>
-      </c>
-      <c r="C45" t="s">
-        <v>256</v>
-      </c>
-      <c r="D45" t="s">
-        <v>7</v>
-      </c>
-      <c r="E45" t="s">
-        <v>184</v>
-      </c>
-      <c r="F45" t="s">
-        <v>253</v>
-      </c>
-      <c r="G45" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="B46" t="s">
-        <v>69</v>
-      </c>
-      <c r="C46" t="s">
-        <v>256</v>
-      </c>
-      <c r="D46" t="s">
-        <v>7</v>
-      </c>
-      <c r="E46" t="s">
-        <v>185</v>
-      </c>
-      <c r="F46" t="s">
-        <v>253</v>
-      </c>
-      <c r="G46" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="B47" t="s">
-        <v>70</v>
-      </c>
-      <c r="C47" t="s">
-        <v>256</v>
-      </c>
-      <c r="D47" t="s">
-        <v>7</v>
-      </c>
-      <c r="E47" t="s">
-        <v>186</v>
-      </c>
-      <c r="F47" t="s">
-        <v>253</v>
-      </c>
-      <c r="G47" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="B48" t="s">
-        <v>71</v>
       </c>
       <c r="C48">
         <v>4</v>
@@ -2335,46 +2377,46 @@
         <v>7</v>
       </c>
       <c r="E48" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F48" t="s">
+        <v>250</v>
+      </c>
+      <c r="G48" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C49" t="s">
         <v>253</v>
       </c>
-      <c r="G48" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="B49" t="s">
-        <v>72</v>
-      </c>
-      <c r="C49" t="s">
-        <v>256</v>
-      </c>
       <c r="D49" t="s">
         <v>7</v>
       </c>
       <c r="E49" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F49" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G49" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C50">
         <v>3</v>
@@ -2383,22 +2425,22 @@
         <v>7</v>
       </c>
       <c r="E50" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F50" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G50" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C51">
         <v>2</v>
@@ -2407,46 +2449,46 @@
         <v>7</v>
       </c>
       <c r="E51" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F51" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G51" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>72</v>
+      </c>
+      <c r="C52" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="52" spans="1:7">
-      <c r="A52">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-      <c r="B52" t="s">
-        <v>75</v>
-      </c>
-      <c r="C52" t="s">
-        <v>257</v>
-      </c>
       <c r="D52" t="s">
         <v>7</v>
       </c>
       <c r="E52" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F52" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G52" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C53">
         <v>5</v>
@@ -2455,22 +2497,22 @@
         <v>7</v>
       </c>
       <c r="E53" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F53" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G53" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C54">
         <v>4</v>
@@ -2482,22 +2524,22 @@
         <v>10</v>
       </c>
       <c r="F54" t="s">
+        <v>250</v>
+      </c>
+      <c r="G54" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>75</v>
+      </c>
+      <c r="C55" t="s">
         <v>253</v>
-      </c>
-      <c r="G54" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
-      <c r="A55">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="B55" t="s">
-        <v>78</v>
-      </c>
-      <c r="C55" t="s">
-        <v>256</v>
       </c>
       <c r="D55" t="s">
         <v>7</v>
@@ -2506,19 +2548,19 @@
         <v>10</v>
       </c>
       <c r="F55" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G55" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C56">
         <v>3</v>
@@ -2527,94 +2569,94 @@
         <v>7</v>
       </c>
       <c r="E56" t="s">
+        <v>190</v>
+      </c>
+      <c r="F56" t="s">
+        <v>250</v>
+      </c>
+      <c r="G56" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>77</v>
+      </c>
+      <c r="C57" t="s">
+        <v>253</v>
+      </c>
+      <c r="D57" t="s">
+        <v>7</v>
+      </c>
+      <c r="E57" t="s">
+        <v>191</v>
+      </c>
+      <c r="F57" t="s">
+        <v>250</v>
+      </c>
+      <c r="G57" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>78</v>
+      </c>
+      <c r="C58" t="s">
+        <v>255</v>
+      </c>
+      <c r="D58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58" t="s">
+        <v>192</v>
+      </c>
+      <c r="F58" t="s">
+        <v>250</v>
+      </c>
+      <c r="G58" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>79</v>
+      </c>
+      <c r="C59" t="s">
+        <v>253</v>
+      </c>
+      <c r="D59" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" t="s">
         <v>193</v>
       </c>
-      <c r="F56" t="s">
-        <v>253</v>
-      </c>
-      <c r="G56" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
-      <c r="A57">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-      <c r="B57" t="s">
+      <c r="F59" t="s">
+        <v>250</v>
+      </c>
+      <c r="G59" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
         <v>80</v>
-      </c>
-      <c r="C57" t="s">
-        <v>256</v>
-      </c>
-      <c r="D57" t="s">
-        <v>7</v>
-      </c>
-      <c r="E57" t="s">
-        <v>194</v>
-      </c>
-      <c r="F57" t="s">
-        <v>253</v>
-      </c>
-      <c r="G57" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
-      <c r="A58">
-        <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="B58" t="s">
-        <v>81</v>
-      </c>
-      <c r="C58" t="s">
-        <v>258</v>
-      </c>
-      <c r="D58" t="s">
-        <v>7</v>
-      </c>
-      <c r="E58" t="s">
-        <v>195</v>
-      </c>
-      <c r="F58" t="s">
-        <v>253</v>
-      </c>
-      <c r="G58" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
-      <c r="A59">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="B59" t="s">
-        <v>82</v>
-      </c>
-      <c r="C59" t="s">
-        <v>256</v>
-      </c>
-      <c r="D59" t="s">
-        <v>7</v>
-      </c>
-      <c r="E59" t="s">
-        <v>196</v>
-      </c>
-      <c r="F59" t="s">
-        <v>253</v>
-      </c>
-      <c r="G59" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7">
-      <c r="A60">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
-      <c r="B60" t="s">
-        <v>83</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -2623,46 +2665,46 @@
         <v>7</v>
       </c>
       <c r="E60" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F60" t="s">
+        <v>250</v>
+      </c>
+      <c r="G60" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>81</v>
+      </c>
+      <c r="C61" t="s">
         <v>253</v>
       </c>
-      <c r="G60" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7">
-      <c r="A61">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="B61" t="s">
-        <v>84</v>
-      </c>
-      <c r="C61" t="s">
-        <v>256</v>
-      </c>
       <c r="D61" t="s">
         <v>7</v>
       </c>
       <c r="E61" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F61" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G61" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C62">
         <v>4</v>
@@ -2671,22 +2713,22 @@
         <v>7</v>
       </c>
       <c r="E62" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F62" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G62" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C63">
         <v>5</v>
@@ -2695,22 +2737,22 @@
         <v>7</v>
       </c>
       <c r="E63" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F63" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G63" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C64">
         <v>5</v>
@@ -2719,25 +2761,25 @@
         <v>7</v>
       </c>
       <c r="E64" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F64" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G64" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C65" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D65" t="s">
         <v>7</v>
@@ -2746,19 +2788,19 @@
         <v>10</v>
       </c>
       <c r="F65" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G65" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C66">
         <v>5</v>
@@ -2767,22 +2809,22 @@
         <v>7</v>
       </c>
       <c r="E66" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F66" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G66" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C67">
         <v>3</v>
@@ -2791,22 +2833,22 @@
         <v>7</v>
       </c>
       <c r="E67" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F67" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G67" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68">
         <f t="shared" si="0"/>
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C68">
         <v>4</v>
@@ -2815,70 +2857,70 @@
         <v>7</v>
       </c>
       <c r="E68" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F68" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G68" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69">
         <f t="shared" si="0"/>
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C69" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D69" t="s">
         <v>7</v>
       </c>
       <c r="E69" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F69" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G69" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70">
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C70" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D70" t="s">
         <v>7</v>
       </c>
       <c r="E70" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F70" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G70" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C71">
         <v>4</v>
@@ -2887,46 +2929,46 @@
         <v>7</v>
       </c>
       <c r="E71" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F71" t="s">
+        <v>250</v>
+      </c>
+      <c r="G71" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>92</v>
+      </c>
+      <c r="C72" t="s">
         <v>253</v>
       </c>
-      <c r="G71" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7">
-      <c r="A72">
-        <f t="shared" si="0"/>
-        <v>71</v>
-      </c>
-      <c r="B72" t="s">
-        <v>95</v>
-      </c>
-      <c r="C72" t="s">
-        <v>256</v>
-      </c>
       <c r="D72" t="s">
         <v>7</v>
       </c>
       <c r="E72" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F72" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G72" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C73">
         <v>4</v>
@@ -2935,40 +2977,40 @@
         <v>7</v>
       </c>
       <c r="E73" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F73" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G73" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74">
         <f t="shared" si="0"/>
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C74" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D74" t="s">
         <v>7</v>
       </c>
       <c r="E74" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F74" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G74" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75">
         <f t="shared" ref="A75:A120" si="1">A74 + 1</f>
         <v>74</v>
@@ -2983,46 +3025,46 @@
         <v>7</v>
       </c>
       <c r="E75" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F75" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G75" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>95</v>
+      </c>
+      <c r="C76" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="76" spans="1:7">
-      <c r="A76">
-        <f t="shared" si="1"/>
-        <v>75</v>
-      </c>
-      <c r="B76" t="s">
-        <v>98</v>
-      </c>
-      <c r="C76" t="s">
-        <v>257</v>
-      </c>
       <c r="D76" t="s">
         <v>7</v>
       </c>
       <c r="E76" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F76" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G76" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C77">
         <v>4</v>
@@ -3031,94 +3073,94 @@
         <v>7</v>
       </c>
       <c r="E77" t="s">
+        <v>207</v>
+      </c>
+      <c r="F77" t="s">
+        <v>250</v>
+      </c>
+      <c r="G77" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>97</v>
+      </c>
+      <c r="C78" t="s">
+        <v>253</v>
+      </c>
+      <c r="D78" t="s">
+        <v>7</v>
+      </c>
+      <c r="E78" t="s">
+        <v>208</v>
+      </c>
+      <c r="F78" t="s">
+        <v>250</v>
+      </c>
+      <c r="G78" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>98</v>
+      </c>
+      <c r="C79" t="s">
+        <v>255</v>
+      </c>
+      <c r="D79" t="s">
+        <v>7</v>
+      </c>
+      <c r="E79" t="s">
+        <v>209</v>
+      </c>
+      <c r="F79" t="s">
+        <v>250</v>
+      </c>
+      <c r="G79" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>99</v>
+      </c>
+      <c r="C80" t="s">
+        <v>253</v>
+      </c>
+      <c r="D80" t="s">
+        <v>7</v>
+      </c>
+      <c r="E80" t="s">
         <v>210</v>
       </c>
-      <c r="F77" t="s">
-        <v>253</v>
-      </c>
-      <c r="G77" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7">
-      <c r="A78">
-        <f t="shared" si="1"/>
-        <v>77</v>
-      </c>
-      <c r="B78" t="s">
+      <c r="F80" t="s">
+        <v>250</v>
+      </c>
+      <c r="G80" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
         <v>100</v>
-      </c>
-      <c r="C78" t="s">
-        <v>256</v>
-      </c>
-      <c r="D78" t="s">
-        <v>7</v>
-      </c>
-      <c r="E78" t="s">
-        <v>211</v>
-      </c>
-      <c r="F78" t="s">
-        <v>253</v>
-      </c>
-      <c r="G78" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7">
-      <c r="A79">
-        <f t="shared" si="1"/>
-        <v>78</v>
-      </c>
-      <c r="B79" t="s">
-        <v>101</v>
-      </c>
-      <c r="C79" t="s">
-        <v>258</v>
-      </c>
-      <c r="D79" t="s">
-        <v>7</v>
-      </c>
-      <c r="E79" t="s">
-        <v>212</v>
-      </c>
-      <c r="F79" t="s">
-        <v>253</v>
-      </c>
-      <c r="G79" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7">
-      <c r="A80">
-        <f t="shared" si="1"/>
-        <v>79</v>
-      </c>
-      <c r="B80" t="s">
-        <v>102</v>
-      </c>
-      <c r="C80" t="s">
-        <v>256</v>
-      </c>
-      <c r="D80" t="s">
-        <v>7</v>
-      </c>
-      <c r="E80" t="s">
-        <v>213</v>
-      </c>
-      <c r="F80" t="s">
-        <v>253</v>
-      </c>
-      <c r="G80" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7">
-      <c r="A81">
-        <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
-      <c r="B81" t="s">
-        <v>103</v>
       </c>
       <c r="C81">
         <v>5</v>
@@ -3127,46 +3169,46 @@
         <v>7</v>
       </c>
       <c r="E81" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F81" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G81" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>101</v>
+      </c>
+      <c r="C82" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="82" spans="1:7">
-      <c r="A82">
-        <f t="shared" si="1"/>
-        <v>81</v>
-      </c>
-      <c r="B82" t="s">
-        <v>104</v>
-      </c>
-      <c r="C82" t="s">
-        <v>257</v>
-      </c>
       <c r="D82" t="s">
         <v>7</v>
       </c>
       <c r="E82" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F82" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G82" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C83">
         <v>4</v>
@@ -3175,46 +3217,46 @@
         <v>7</v>
       </c>
       <c r="E83" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F83" t="s">
+        <v>250</v>
+      </c>
+      <c r="G83" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>103</v>
+      </c>
+      <c r="C84" t="s">
         <v>253</v>
       </c>
-      <c r="G83" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7">
-      <c r="A84">
-        <f t="shared" si="1"/>
-        <v>83</v>
-      </c>
-      <c r="B84" t="s">
-        <v>106</v>
-      </c>
-      <c r="C84" t="s">
-        <v>256</v>
-      </c>
       <c r="D84" t="s">
         <v>7</v>
       </c>
       <c r="E84" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F84" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G84" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C85">
         <v>3</v>
@@ -3223,22 +3265,22 @@
         <v>7</v>
       </c>
       <c r="E85" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F85" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G85" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86">
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C86">
         <v>4</v>
@@ -3247,46 +3289,46 @@
         <v>7</v>
       </c>
       <c r="E86" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F86" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G86" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>106</v>
+      </c>
+      <c r="C87" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="87" spans="1:7">
-      <c r="A87">
-        <f t="shared" si="1"/>
-        <v>86</v>
-      </c>
-      <c r="B87" t="s">
-        <v>109</v>
-      </c>
-      <c r="C87" t="s">
-        <v>257</v>
-      </c>
       <c r="D87" t="s">
         <v>7</v>
       </c>
       <c r="E87" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F87" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G87" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88">
         <f t="shared" si="1"/>
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C88">
         <v>4</v>
@@ -3295,46 +3337,46 @@
         <v>7</v>
       </c>
       <c r="E88" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F88" t="s">
+        <v>250</v>
+      </c>
+      <c r="G88" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>108</v>
+      </c>
+      <c r="C89" t="s">
         <v>253</v>
       </c>
-      <c r="G88" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7">
-      <c r="A89">
-        <f t="shared" si="1"/>
-        <v>88</v>
-      </c>
-      <c r="B89" t="s">
-        <v>111</v>
-      </c>
-      <c r="C89" t="s">
-        <v>256</v>
-      </c>
       <c r="D89" t="s">
         <v>7</v>
       </c>
       <c r="E89" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F89" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G89" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90">
         <f t="shared" si="1"/>
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C90">
         <v>3</v>
@@ -3343,22 +3385,22 @@
         <v>7</v>
       </c>
       <c r="E90" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F90" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G90" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C91">
         <v>4</v>
@@ -3367,94 +3409,94 @@
         <v>7</v>
       </c>
       <c r="E91" t="s">
+        <v>221</v>
+      </c>
+      <c r="F91" t="s">
+        <v>250</v>
+      </c>
+      <c r="G91" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>111</v>
+      </c>
+      <c r="C92" t="s">
+        <v>255</v>
+      </c>
+      <c r="D92" t="s">
+        <v>7</v>
+      </c>
+      <c r="E92" t="s">
+        <v>222</v>
+      </c>
+      <c r="F92" t="s">
+        <v>250</v>
+      </c>
+      <c r="G92" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>112</v>
+      </c>
+      <c r="C93" t="s">
+        <v>253</v>
+      </c>
+      <c r="D93" t="s">
+        <v>7</v>
+      </c>
+      <c r="E93" t="s">
+        <v>223</v>
+      </c>
+      <c r="F93" t="s">
+        <v>250</v>
+      </c>
+      <c r="G93" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>113</v>
+      </c>
+      <c r="C94" t="s">
+        <v>253</v>
+      </c>
+      <c r="D94" t="s">
+        <v>7</v>
+      </c>
+      <c r="E94" t="s">
         <v>224</v>
       </c>
-      <c r="F91" t="s">
-        <v>253</v>
-      </c>
-      <c r="G91" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7">
-      <c r="A92">
-        <f t="shared" si="1"/>
-        <v>91</v>
-      </c>
-      <c r="B92" t="s">
+      <c r="F94" t="s">
+        <v>250</v>
+      </c>
+      <c r="G94" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
         <v>114</v>
-      </c>
-      <c r="C92" t="s">
-        <v>258</v>
-      </c>
-      <c r="D92" t="s">
-        <v>7</v>
-      </c>
-      <c r="E92" t="s">
-        <v>225</v>
-      </c>
-      <c r="F92" t="s">
-        <v>253</v>
-      </c>
-      <c r="G92" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7">
-      <c r="A93">
-        <f t="shared" si="1"/>
-        <v>92</v>
-      </c>
-      <c r="B93" t="s">
-        <v>115</v>
-      </c>
-      <c r="C93" t="s">
-        <v>256</v>
-      </c>
-      <c r="D93" t="s">
-        <v>7</v>
-      </c>
-      <c r="E93" t="s">
-        <v>226</v>
-      </c>
-      <c r="F93" t="s">
-        <v>253</v>
-      </c>
-      <c r="G93" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7">
-      <c r="A94">
-        <f t="shared" si="1"/>
-        <v>93</v>
-      </c>
-      <c r="B94" t="s">
-        <v>116</v>
-      </c>
-      <c r="C94" t="s">
-        <v>256</v>
-      </c>
-      <c r="D94" t="s">
-        <v>7</v>
-      </c>
-      <c r="E94" t="s">
-        <v>227</v>
-      </c>
-      <c r="F94" t="s">
-        <v>253</v>
-      </c>
-      <c r="G94" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7">
-      <c r="A95">
-        <f t="shared" si="1"/>
-        <v>94</v>
-      </c>
-      <c r="B95" t="s">
-        <v>117</v>
       </c>
       <c r="C95">
         <v>4</v>
@@ -3463,70 +3505,70 @@
         <v>7</v>
       </c>
       <c r="E95" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F95" t="s">
+        <v>250</v>
+      </c>
+      <c r="G95" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>115</v>
+      </c>
+      <c r="C96" t="s">
         <v>253</v>
       </c>
-      <c r="G95" t="s">
+      <c r="D96" t="s">
+        <v>7</v>
+      </c>
+      <c r="E96" t="s">
+        <v>226</v>
+      </c>
+      <c r="F96" t="s">
+        <v>250</v>
+      </c>
+      <c r="G96" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>116</v>
+      </c>
+      <c r="C97" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="96" spans="1:7">
-      <c r="A96">
-        <f t="shared" si="1"/>
-        <v>95</v>
-      </c>
-      <c r="B96" t="s">
-        <v>118</v>
-      </c>
-      <c r="C96" t="s">
-        <v>256</v>
-      </c>
-      <c r="D96" t="s">
-        <v>7</v>
-      </c>
-      <c r="E96" t="s">
-        <v>229</v>
-      </c>
-      <c r="F96" t="s">
-        <v>253</v>
-      </c>
-      <c r="G96" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7">
-      <c r="A97">
-        <f t="shared" si="1"/>
-        <v>96</v>
-      </c>
-      <c r="B97" t="s">
-        <v>119</v>
-      </c>
-      <c r="C97" t="s">
-        <v>257</v>
-      </c>
       <c r="D97" t="s">
         <v>7</v>
       </c>
       <c r="E97" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F97" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G97" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98">
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C98">
         <v>4</v>
@@ -3535,22 +3577,22 @@
         <v>7</v>
       </c>
       <c r="E98" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F98" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G98" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C99">
         <v>5</v>
@@ -3559,46 +3601,46 @@
         <v>7</v>
       </c>
       <c r="E99" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F99" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G99" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>119</v>
+      </c>
+      <c r="C100" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="100" spans="1:7">
-      <c r="A100">
-        <f t="shared" si="1"/>
-        <v>99</v>
-      </c>
-      <c r="B100" t="s">
-        <v>122</v>
-      </c>
-      <c r="C100" t="s">
-        <v>257</v>
-      </c>
       <c r="D100" t="s">
         <v>7</v>
       </c>
       <c r="E100" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F100" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G100" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C101">
         <v>4</v>
@@ -3607,22 +3649,22 @@
         <v>7</v>
       </c>
       <c r="E101" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F101" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G101" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C102">
         <v>4</v>
@@ -3631,94 +3673,94 @@
         <v>7</v>
       </c>
       <c r="E102" t="s">
+        <v>232</v>
+      </c>
+      <c r="F102" t="s">
+        <v>250</v>
+      </c>
+      <c r="G102" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
+        <v>122</v>
+      </c>
+      <c r="C103" t="s">
+        <v>253</v>
+      </c>
+      <c r="D103" t="s">
+        <v>7</v>
+      </c>
+      <c r="E103" t="s">
+        <v>233</v>
+      </c>
+      <c r="F103" t="s">
+        <v>250</v>
+      </c>
+      <c r="G103" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <f t="shared" si="1"/>
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
+        <v>123</v>
+      </c>
+      <c r="C104" t="s">
+        <v>253</v>
+      </c>
+      <c r="D104" t="s">
+        <v>7</v>
+      </c>
+      <c r="E104" t="s">
+        <v>234</v>
+      </c>
+      <c r="F104" t="s">
+        <v>250</v>
+      </c>
+      <c r="G104" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="B105" t="s">
+        <v>124</v>
+      </c>
+      <c r="C105" t="s">
+        <v>253</v>
+      </c>
+      <c r="D105" t="s">
+        <v>7</v>
+      </c>
+      <c r="E105" t="s">
         <v>235</v>
       </c>
-      <c r="F102" t="s">
-        <v>253</v>
-      </c>
-      <c r="G102" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7">
-      <c r="A103">
-        <f t="shared" si="1"/>
-        <v>102</v>
-      </c>
-      <c r="B103" t="s">
+      <c r="F105" t="s">
+        <v>250</v>
+      </c>
+      <c r="G105" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="B106" t="s">
         <v>125</v>
-      </c>
-      <c r="C103" t="s">
-        <v>256</v>
-      </c>
-      <c r="D103" t="s">
-        <v>7</v>
-      </c>
-      <c r="E103" t="s">
-        <v>236</v>
-      </c>
-      <c r="F103" t="s">
-        <v>253</v>
-      </c>
-      <c r="G103" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7">
-      <c r="A104">
-        <f t="shared" si="1"/>
-        <v>103</v>
-      </c>
-      <c r="B104" t="s">
-        <v>126</v>
-      </c>
-      <c r="C104" t="s">
-        <v>256</v>
-      </c>
-      <c r="D104" t="s">
-        <v>7</v>
-      </c>
-      <c r="E104" t="s">
-        <v>237</v>
-      </c>
-      <c r="F104" t="s">
-        <v>253</v>
-      </c>
-      <c r="G104" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7">
-      <c r="A105">
-        <f t="shared" si="1"/>
-        <v>104</v>
-      </c>
-      <c r="B105" t="s">
-        <v>127</v>
-      </c>
-      <c r="C105" t="s">
-        <v>256</v>
-      </c>
-      <c r="D105" t="s">
-        <v>7</v>
-      </c>
-      <c r="E105" t="s">
-        <v>238</v>
-      </c>
-      <c r="F105" t="s">
-        <v>253</v>
-      </c>
-      <c r="G105" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7">
-      <c r="A106">
-        <f t="shared" si="1"/>
-        <v>105</v>
-      </c>
-      <c r="B106" t="s">
-        <v>128</v>
       </c>
       <c r="C106">
         <v>4</v>
@@ -3727,46 +3769,46 @@
         <v>7</v>
       </c>
       <c r="E106" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F106" t="s">
+        <v>250</v>
+      </c>
+      <c r="G106" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+      <c r="B107" t="s">
+        <v>126</v>
+      </c>
+      <c r="C107" t="s">
         <v>253</v>
       </c>
-      <c r="G106" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7">
-      <c r="A107">
-        <f t="shared" si="1"/>
-        <v>106</v>
-      </c>
-      <c r="B107" t="s">
-        <v>129</v>
-      </c>
-      <c r="C107" t="s">
-        <v>256</v>
-      </c>
       <c r="D107" t="s">
         <v>7</v>
       </c>
       <c r="E107" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F107" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G107" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108">
         <f t="shared" si="1"/>
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C108">
         <v>4</v>
@@ -3775,22 +3817,22 @@
         <v>7</v>
       </c>
       <c r="E108" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F108" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G108" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109">
         <f t="shared" si="1"/>
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C109">
         <v>3</v>
@@ -3799,22 +3841,22 @@
         <v>7</v>
       </c>
       <c r="E109" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="F109" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G109" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110">
         <f t="shared" si="1"/>
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C110">
         <v>5</v>
@@ -3823,142 +3865,142 @@
         <v>7</v>
       </c>
       <c r="E110" t="s">
+        <v>240</v>
+      </c>
+      <c r="F110" t="s">
+        <v>250</v>
+      </c>
+      <c r="G110" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="B111" t="s">
+        <v>130</v>
+      </c>
+      <c r="C111" t="s">
+        <v>254</v>
+      </c>
+      <c r="D111" t="s">
+        <v>7</v>
+      </c>
+      <c r="E111" t="s">
+        <v>241</v>
+      </c>
+      <c r="F111" t="s">
+        <v>250</v>
+      </c>
+      <c r="G111" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <f t="shared" si="1"/>
+        <v>111</v>
+      </c>
+      <c r="B112" t="s">
+        <v>131</v>
+      </c>
+      <c r="C112" t="s">
+        <v>254</v>
+      </c>
+      <c r="D112" t="s">
+        <v>7</v>
+      </c>
+      <c r="E112" t="s">
+        <v>242</v>
+      </c>
+      <c r="F112" t="s">
+        <v>250</v>
+      </c>
+      <c r="G112" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="B113" t="s">
+        <v>132</v>
+      </c>
+      <c r="C113" t="s">
+        <v>253</v>
+      </c>
+      <c r="D113" t="s">
+        <v>7</v>
+      </c>
+      <c r="E113" t="s">
         <v>243</v>
       </c>
-      <c r="F110" t="s">
+      <c r="F113" t="s">
+        <v>250</v>
+      </c>
+      <c r="G113" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
+      <c r="B114" t="s">
+        <v>133</v>
+      </c>
+      <c r="C114" t="s">
         <v>253</v>
       </c>
-      <c r="G110" t="s">
+      <c r="D114" t="s">
+        <v>7</v>
+      </c>
+      <c r="E114" t="s">
+        <v>244</v>
+      </c>
+      <c r="F114" t="s">
+        <v>250</v>
+      </c>
+      <c r="G114" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <f t="shared" si="1"/>
+        <v>114</v>
+      </c>
+      <c r="B115" t="s">
+        <v>134</v>
+      </c>
+      <c r="C115" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="111" spans="1:7">
-      <c r="A111">
-        <f t="shared" si="1"/>
-        <v>110</v>
-      </c>
-      <c r="B111" t="s">
-        <v>133</v>
-      </c>
-      <c r="C111" t="s">
-        <v>257</v>
-      </c>
-      <c r="D111" t="s">
-        <v>7</v>
-      </c>
-      <c r="E111" t="s">
-        <v>244</v>
-      </c>
-      <c r="F111" t="s">
-        <v>253</v>
-      </c>
-      <c r="G111" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7">
-      <c r="A112">
-        <f t="shared" si="1"/>
-        <v>111</v>
-      </c>
-      <c r="B112" t="s">
-        <v>134</v>
-      </c>
-      <c r="C112" t="s">
-        <v>257</v>
-      </c>
-      <c r="D112" t="s">
-        <v>7</v>
-      </c>
-      <c r="E112" t="s">
+      <c r="D115" t="s">
+        <v>7</v>
+      </c>
+      <c r="E115" t="s">
         <v>245</v>
       </c>
-      <c r="F112" t="s">
-        <v>253</v>
-      </c>
-      <c r="G112" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7">
-      <c r="A113">
-        <f t="shared" si="1"/>
-        <v>112</v>
-      </c>
-      <c r="B113" t="s">
+      <c r="F115" t="s">
+        <v>250</v>
+      </c>
+      <c r="G115" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <f t="shared" si="1"/>
+        <v>115</v>
+      </c>
+      <c r="B116" t="s">
         <v>135</v>
-      </c>
-      <c r="C113" t="s">
-        <v>256</v>
-      </c>
-      <c r="D113" t="s">
-        <v>7</v>
-      </c>
-      <c r="E113" t="s">
-        <v>246</v>
-      </c>
-      <c r="F113" t="s">
-        <v>253</v>
-      </c>
-      <c r="G113" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7">
-      <c r="A114">
-        <f t="shared" si="1"/>
-        <v>113</v>
-      </c>
-      <c r="B114" t="s">
-        <v>136</v>
-      </c>
-      <c r="C114" t="s">
-        <v>256</v>
-      </c>
-      <c r="D114" t="s">
-        <v>7</v>
-      </c>
-      <c r="E114" t="s">
-        <v>247</v>
-      </c>
-      <c r="F114" t="s">
-        <v>253</v>
-      </c>
-      <c r="G114" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7">
-      <c r="A115">
-        <f t="shared" si="1"/>
-        <v>114</v>
-      </c>
-      <c r="B115" t="s">
-        <v>137</v>
-      </c>
-      <c r="C115" t="s">
-        <v>257</v>
-      </c>
-      <c r="D115" t="s">
-        <v>7</v>
-      </c>
-      <c r="E115" t="s">
-        <v>248</v>
-      </c>
-      <c r="F115" t="s">
-        <v>253</v>
-      </c>
-      <c r="G115" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7">
-      <c r="A116">
-        <f t="shared" si="1"/>
-        <v>115</v>
-      </c>
-      <c r="B116" t="s">
-        <v>138</v>
       </c>
       <c r="C116">
         <v>4</v>
@@ -3967,22 +4009,22 @@
         <v>7</v>
       </c>
       <c r="E116" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F116" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G116" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117">
         <f t="shared" si="1"/>
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C117">
         <v>4</v>
@@ -3991,22 +4033,22 @@
         <v>7</v>
       </c>
       <c r="E117" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F117" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G117" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118">
         <f t="shared" si="1"/>
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C118">
         <v>4</v>
@@ -4015,22 +4057,22 @@
         <v>7</v>
       </c>
       <c r="E118" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F118" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G118" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119">
         <f t="shared" si="1"/>
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C119">
         <v>4</v>
@@ -4039,37 +4081,37 @@
         <v>7</v>
       </c>
       <c r="E119" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F119" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G119" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <f t="shared" si="1"/>
+        <v>119</v>
+      </c>
+      <c r="B120" t="s">
+        <v>139</v>
+      </c>
+      <c r="C120" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="120" spans="1:7">
-      <c r="A120">
-        <f t="shared" si="1"/>
-        <v>119</v>
-      </c>
-      <c r="B120" t="s">
-        <v>142</v>
-      </c>
-      <c r="C120" t="s">
-        <v>257</v>
-      </c>
       <c r="D120" t="s">
         <v>7</v>
       </c>
       <c r="E120" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F120" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G120" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>